<commit_message>
Realised order import from xlsx
</commit_message>
<xml_diff>
--- a/shoe_store/import_data/order_import.xlsx
+++ b/shoe_store/import_data/order_import.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Новая папка (2)\Пример\import\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data\my_garbage\demka_project\shoe_store\import_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B417337-0A44-41F9-AFF0-E4A62BDEE9DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="1020" windowWidth="17280" windowHeight="9420"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -19,18 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="20">
   <si>
     <t>Номер заказа</t>
   </si>
@@ -90,15 +85,12 @@
   </si>
   <si>
     <t>S213E3, 5, E482R4, 5</t>
-  </si>
-  <si>
-    <t>30.02.2025</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4">
     <font>
       <sz val="12"/>
@@ -498,11 +490,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -735,8 +727,8 @@
       <c r="B8" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="6" t="s">
-        <v>20</v>
+      <c r="C8" s="6">
+        <v>45716</v>
       </c>
       <c r="D8" s="6">
         <v>45773</v>

</xml_diff>